<commit_message>
Almost 3 types are done
</commit_message>
<xml_diff>
--- a/WATER LUPA/acea-water-prediction/New folder/datasets_description.xlsx
+++ b/WATER LUPA/acea-water-prediction/New folder/datasets_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antimo.Musone\OneDrive - EY\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\MACHINE LEARNING\1810026_ECE4100_IndustialTraining\WATER LUPA\acea-water-prediction\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{A47BE5A7-D45A-4BB1-AE49-E6FCEE3550AB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{BA5CFFF6-35E3-451A-A08E-1D368B0185A6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2EEB5D-E595-442B-A5A0-05999BFE362B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58D5F0AE-44AF-4F76-9ADB-3D5614CBD446}"/>
+    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="12504" xr2:uid="{58D5F0AE-44AF-4F76-9ADB-3D5614CBD446}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets_Description" sheetId="1" r:id="rId1"/>
@@ -1169,7 +1169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1184,10 +1184,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2032,8 +2028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D2189E-1773-48E7-BBD0-CE742FBAD0D6}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2312,36 +2308,33 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="7" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -2351,11 +2344,8 @@
       <c r="C12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-    </row>
-    <row r="13" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -2365,9 +2355,6 @@
       <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
       <c r="G13" s="1" t="s">
         <v>9</v>
       </c>
@@ -2375,7 +2362,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>49</v>
       </c>
@@ -2385,9 +2372,6 @@
       <c r="C14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
       <c r="G14" s="3" t="s">
         <v>11</v>
       </c>
@@ -2395,7 +2379,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -2405,9 +2389,6 @@
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
       <c r="G15" s="3" t="s">
         <v>16</v>
       </c>
@@ -2415,7 +2396,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
@@ -2425,9 +2406,6 @@
       <c r="C16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
       <c r="G16" s="3" t="s">
         <v>17</v>
       </c>
@@ -2435,7 +2413,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
@@ -2445,9 +2423,6 @@
       <c r="C17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
       <c r="G17" s="3" t="s">
         <v>20</v>
       </c>
@@ -2455,36 +2430,33 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="7" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>63</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -2494,11 +2466,8 @@
       <c r="C21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-    </row>
-    <row r="22" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>13</v>
       </c>
@@ -2508,9 +2477,6 @@
       <c r="C22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
       <c r="G22" s="1" t="s">
         <v>9</v>
       </c>
@@ -2518,7 +2484,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
@@ -2528,9 +2494,6 @@
       <c r="C23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
       <c r="G23" s="3" t="s">
         <v>11</v>
       </c>
@@ -2538,7 +2501,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
@@ -2548,9 +2511,6 @@
       <c r="C24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
       <c r="G24" s="3" t="s">
         <v>16</v>
       </c>
@@ -2558,7 +2518,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -2568,9 +2528,6 @@
       <c r="C25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
       <c r="G25" s="3" t="s">
         <v>17</v>
       </c>
@@ -2578,7 +2535,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>60</v>
       </c>
@@ -2588,9 +2545,6 @@
       <c r="C26" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
       <c r="G26" s="3" t="s">
         <v>20</v>
       </c>
@@ -2598,14 +2552,14 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="1" t="s">
         <v>126</v>
       </c>
       <c r="G27" s="3" t="s">
@@ -2616,35 +2570,32 @@
       </c>
     </row>
     <row r="28" spans="1:8" s="5" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-    </row>
-    <row r="29" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-    </row>
-    <row r="30" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
@@ -2654,11 +2605,8 @@
       <c r="C31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-    </row>
-    <row r="32" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>13</v>
       </c>
@@ -2668,9 +2616,6 @@
       <c r="C32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D32"/>
-      <c r="E32"/>
-      <c r="F32"/>
       <c r="G32" s="1" t="s">
         <v>9</v>
       </c>
@@ -2678,7 +2623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>49</v>
       </c>
@@ -2688,9 +2633,6 @@
       <c r="C33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
       <c r="G33" s="3" t="s">
         <v>11</v>
       </c>
@@ -2698,7 +2640,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>50</v>
       </c>
@@ -2708,9 +2650,6 @@
       <c r="C34" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
       <c r="G34" s="3" t="s">
         <v>16</v>
       </c>
@@ -2718,7 +2657,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>51</v>
       </c>
@@ -2728,9 +2667,6 @@
       <c r="C35" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D35"/>
-      <c r="E35"/>
-      <c r="F35"/>
       <c r="G35" s="3" t="s">
         <v>17</v>
       </c>
@@ -2738,7 +2674,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
@@ -2748,9 +2684,6 @@
       <c r="C36" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D36"/>
-      <c r="E36"/>
-      <c r="F36"/>
       <c r="G36" s="3" t="s">
         <v>20</v>
       </c>
@@ -2758,22 +2691,22 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="6"/>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
+      <c r="C37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" s="5" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
@@ -2888,14 +2821,14 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
@@ -2982,14 +2915,14 @@
       </c>
     </row>
     <row r="55" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="8"/>
-      <c r="H55" s="8"/>
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
@@ -3081,20 +3014,20 @@
       <c r="C63" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F63" s="10"/>
-      <c r="G63" s="10"/>
-      <c r="H63" s="10"/>
-      <c r="I63" s="10"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
     </row>
     <row r="64" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="8"/>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="8"/>
-      <c r="H64" s="8"/>
+      <c r="A64" s="6"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
@@ -3164,14 +3097,14 @@
       </c>
     </row>
     <row r="71" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="8"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="9"/>
-      <c r="E71" s="9"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8"/>
+      <c r="A71" s="6"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
@@ -3261,9 +3194,9 @@
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
-      <c r="F79" s="10"/>
-      <c r="G79" s="10"/>
-      <c r="H79" s="10"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3309,41 +3242,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
+      <c r="A3" s="16"/>
       <c r="B3" t="s">
         <v>113</v>
       </c>
@@ -3353,12 +3286,12 @@
       <c r="D3" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
+      <c r="A4" s="16"/>
       <c r="B4" t="s">
         <v>114</v>
       </c>
@@ -3368,12 +3301,12 @@
       <c r="D4" t="s">
         <v>111</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="12" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
+      <c r="A5" s="16"/>
       <c r="B5" t="s">
         <v>115</v>
       </c>
@@ -3383,27 +3316,27 @@
       <c r="D5" t="s">
         <v>111</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="E6" s="16" t="s">
+      <c r="C6" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="16" t="s">
         <v>57</v>
       </c>
       <c r="B7" t="s">
@@ -3415,13 +3348,13 @@
       <c r="D7" t="s">
         <v>112</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
-      <c r="B8" s="17" t="s">
+      <c r="A8" s="16"/>
+      <c r="B8" s="15" t="s">
         <v>117</v>
       </c>
       <c r="C8" t="s">
@@ -3430,12 +3363,12 @@
       <c r="D8" t="s">
         <v>112</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
+      <c r="A9" s="16"/>
       <c r="B9" t="s">
         <v>114</v>
       </c>
@@ -3445,27 +3378,27 @@
       <c r="D9" t="s">
         <v>111</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="12" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="19"/>
-      <c r="B10" s="15" t="s">
+      <c r="A10" s="17"/>
+      <c r="B10" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" s="15" t="s">
+      <c r="C10" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="14" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B11" t="s">
@@ -3477,12 +3410,12 @@
       <c r="D11" t="s">
         <v>112</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
+      <c r="A12" s="16"/>
       <c r="B12" t="s">
         <v>113</v>
       </c>
@@ -3492,12 +3425,12 @@
       <c r="D12" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
+      <c r="A13" s="16"/>
       <c r="B13" t="s">
         <v>114</v>
       </c>
@@ -3507,12 +3440,12 @@
       <c r="D13" t="s">
         <v>111</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="12" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
+      <c r="A14" s="16"/>
       <c r="B14" t="s">
         <v>118</v>
       </c>
@@ -3522,27 +3455,27 @@
       <c r="D14" t="s">
         <v>111</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
-      <c r="B15" s="15" t="s">
+      <c r="A15" s="17"/>
+      <c r="B15" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="E15" s="16" t="s">
+      <c r="C15" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="14" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="16" t="s">
         <v>71</v>
       </c>
       <c r="B16" t="s">
@@ -3554,12 +3487,12 @@
       <c r="D16" t="s">
         <v>112</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
+      <c r="A17" s="16"/>
       <c r="B17" t="s">
         <v>113</v>
       </c>
@@ -3569,12 +3502,12 @@
       <c r="D17" t="s">
         <v>111</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
+      <c r="A18" s="16"/>
       <c r="B18" t="s">
         <v>114</v>
       </c>
@@ -3584,27 +3517,27 @@
       <c r="D18" t="s">
         <v>111</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="12" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="17"/>
+      <c r="B19" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="E19" s="16" t="s">
+      <c r="D19" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B20" t="s">
@@ -3616,12 +3549,12 @@
       <c r="D20" t="s">
         <v>112</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
+      <c r="A21" s="16"/>
       <c r="B21" t="s">
         <v>113</v>
       </c>
@@ -3631,12 +3564,12 @@
       <c r="D21" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
+      <c r="A22" s="16"/>
       <c r="B22" t="s">
         <v>114</v>
       </c>
@@ -3646,27 +3579,27 @@
       <c r="D22" t="s">
         <v>111</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="12" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="19"/>
-      <c r="B23" s="15" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D23" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="E23" s="16" t="s">
+      <c r="D23" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="14" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B24" t="s">
@@ -3678,12 +3611,12 @@
       <c r="D24" t="s">
         <v>112</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
+      <c r="A25" s="16"/>
       <c r="B25" t="s">
         <v>121</v>
       </c>
@@ -3693,27 +3626,27 @@
       <c r="D25" t="s">
         <v>111</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="12" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="19"/>
-      <c r="B26" s="15" t="s">
+      <c r="A26" s="17"/>
+      <c r="B26" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="E26" s="16" t="s">
+      <c r="C26" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="14" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B27" t="s">
@@ -3725,12 +3658,12 @@
       <c r="D27" t="s">
         <v>112</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="18"/>
+      <c r="A28" s="16"/>
       <c r="B28" t="s">
         <v>121</v>
       </c>
@@ -3740,12 +3673,12 @@
       <c r="D28" t="s">
         <v>111</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="12" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="18"/>
+      <c r="A29" s="16"/>
       <c r="B29" t="s">
         <v>42</v>
       </c>
@@ -3755,27 +3688,27 @@
       <c r="D29" t="s">
         <v>112</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="19"/>
-      <c r="B30" s="15" t="s">
+      <c r="A30" s="17"/>
+      <c r="B30" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="D30" s="15" t="s">
+      <c r="C30" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="14" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="16" t="s">
         <v>91</v>
       </c>
       <c r="B31" t="s">
@@ -3787,27 +3720,27 @@
       <c r="D31" t="s">
         <v>112</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="19"/>
-      <c r="B32" s="15" t="s">
+      <c r="A32" s="17"/>
+      <c r="B32" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D32" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="E32" s="16" t="s">
+      <c r="D32" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32" s="14" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="16" t="s">
         <v>124</v>
       </c>
       <c r="B33" t="s">
@@ -3819,12 +3752,12 @@
       <c r="D33" t="s">
         <v>112</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="18"/>
+      <c r="A34" s="16"/>
       <c r="B34" t="s">
         <v>121</v>
       </c>
@@ -3834,22 +3767,22 @@
       <c r="D34" t="s">
         <v>111</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="12" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="19"/>
-      <c r="B35" s="15" t="s">
+      <c r="A35" s="17"/>
+      <c r="B35" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="C35" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="D35" s="15" t="s">
+      <c r="C35" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="E35" s="16" t="s">
+      <c r="E35" s="14" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3870,6 +3803,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A2CE81D0E9067B4C9491F29EF2260D9A" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5b5f5cf789d994f288cb530aae4d4947">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1ee2afc6-efc0-4dcc-be09-aabefb754106" xmlns:ns4="6dff4707-7bf8-4102-b125-42e04ae9fdfc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="86a904f73a016299fbde656704a2a3dc" ns3:_="" ns4:_="">
     <xsd:import namespace="1ee2afc6-efc0-4dcc-be09-aabefb754106"/>
@@ -4092,22 +4040,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B65F2D0C-2F4F-423E-93D0-474B015820DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1ee2afc6-efc0-4dcc-be09-aabefb754106"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6dff4707-7bf8-4102-b125-42e04ae9fdfc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79FC5E73-FF93-4287-85E1-280261870305}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24A7BAD6-613C-4DC5-B7D4-D945ED99237C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4124,29 +4082,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79FC5E73-FF93-4287-85E1-280261870305}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B65F2D0C-2F4F-423E-93D0-474B015820DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1ee2afc6-efc0-4dcc-be09-aabefb754106"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6dff4707-7bf8-4102-b125-42e04ae9fdfc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>